<commit_message>
xlsx json send is wroking
</commit_message>
<xml_diff>
--- a/server/uploads/spreadsheets/fakedata.xlsx
+++ b/server/uploads/spreadsheets/fakedata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\Programming2022\headstarter-resume-parser\resumes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\Programming2022\headstarter-resume-parser-group-project\server\uploads\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{096B7D35-30CA-4E12-B6A2-2FF45850412A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B848CB7-4914-4FC1-97BE-9F04D263F4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6615" yWindow="2400" windowWidth="21600" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7005" yWindow="765" windowWidth="21600" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
   <si>
     <t>id</t>
   </si>
@@ -167,6 +167,69 @@
   </si>
   <si>
     <t>SQL</t>
+  </si>
+  <si>
+    <t>rsnoding0@marketwatch.com</t>
+  </si>
+  <si>
+    <t>glamprey1@tmall.com</t>
+  </si>
+  <si>
+    <t>zloosemore2@nymag.com</t>
+  </si>
+  <si>
+    <t>mflaunders3@behance.net</t>
+  </si>
+  <si>
+    <t>mlarkkem4@cafepress.com</t>
+  </si>
+  <si>
+    <t>mcoopper5@cisco.com</t>
+  </si>
+  <si>
+    <t>grandales6@networksolutions.com</t>
+  </si>
+  <si>
+    <t>lbreyt7@goo.ne.jp</t>
+  </si>
+  <si>
+    <t>mfern8@salon.com</t>
+  </si>
+  <si>
+    <t>check9@networksolutions.com</t>
+  </si>
+  <si>
+    <t>condruseka@nbcnews.com</t>
+  </si>
+  <si>
+    <t>mgerattb@weather.com</t>
+  </si>
+  <si>
+    <t>ccastelc@kickstarter.com</t>
+  </si>
+  <si>
+    <t>cmissendend@java.com</t>
+  </si>
+  <si>
+    <t>predholee@vinaora.com</t>
+  </si>
+  <si>
+    <t>pmateosf@illinois.edu</t>
+  </si>
+  <si>
+    <t>lrodenburgg@pcworld.com</t>
+  </si>
+  <si>
+    <t>cmonginh@goo.ne.jp</t>
+  </si>
+  <si>
+    <t>bjumeaui@google.ru</t>
+  </si>
+  <si>
+    <t>mhammandj@independent.co.uk</t>
+  </si>
+  <si>
+    <t>contact</t>
   </si>
 </sst>
 </file>
@@ -200,8 +263,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="E2" sqref="E2:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -528,10 +594,11 @@
     <col min="2" max="2" width="9.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.375" customWidth="1"/>
+    <col min="6" max="6" width="70.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -547,8 +614,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -564,8 +634,11 @@
       <c r="E2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -581,8 +654,11 @@
       <c r="E3">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -598,8 +674,11 @@
       <c r="E4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -615,8 +694,11 @@
       <c r="E5">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -632,8 +714,11 @@
       <c r="E6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -649,8 +734,11 @@
       <c r="E7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -666,8 +754,11 @@
       <c r="E8">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -683,8 +774,11 @@
       <c r="E9">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -700,8 +794,11 @@
       <c r="E10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -717,8 +814,11 @@
       <c r="E11">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -734,8 +834,11 @@
       <c r="E12">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -751,8 +854,11 @@
       <c r="E13">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -768,8 +874,11 @@
       <c r="E14">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -785,8 +894,11 @@
       <c r="E15">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -802,8 +914,11 @@
       <c r="E16">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -819,8 +934,11 @@
       <c r="E17">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -836,8 +954,11 @@
       <c r="E18">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -853,8 +974,11 @@
       <c r="E19">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -870,8 +994,11 @@
       <c r="E20">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -886,6 +1013,9 @@
       </c>
       <c r="E21">
         <v>11</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>